<commit_message>
Added files and changed structure
</commit_message>
<xml_diff>
--- a/Data/Per RHA/PIB.xlsx
+++ b/Data/Per RHA/PIB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charly\Documents\Data Science\Projects\Water management\Data\Per RHA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\charlyfive\Documents\Projects\water_management\Data\Per RHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A0009-86E3-42DF-BC28-BD5DDB100C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDC9AE8-4B5D-4EAC-A01A-078B3E7FDE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18450" yWindow="5055" windowWidth="27960" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>I</t>
   </si>
@@ -120,19 +120,13 @@
   </si>
   <si>
     <t xml:space="preserve">Nombre </t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,12 +148,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -240,12 +228,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -528,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,86 +1190,6 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
     </row>
-    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" ref="C15:Q15" si="0">SUM(C2:C14)</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
-        <f t="shared" si="0"/>
-        <v>99.990000000000023</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <f t="shared" si="0"/>
-        <v>99.99</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="0"/>
-        <v>100.02</v>
-      </c>
-      <c r="J15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <f t="shared" si="0"/>
-        <v>99.98</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="0"/>
-        <v>99.990000000000009</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="0"/>
-        <v>100.01</v>
-      </c>
-      <c r="N15" s="7">
-        <f t="shared" si="0"/>
-        <v>99.999999999999986</v>
-      </c>
-      <c r="O15" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="P15" s="7">
-        <f t="shared" si="0"/>
-        <v>100.00999999999999</v>
-      </c>
-      <c r="Q15" s="7">
-        <f t="shared" si="0"/>
-        <v>100.00000000000001</v>
-      </c>
-      <c r="R15" s="7">
-        <f>SUM(R2:R14)</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="7">
-        <f t="shared" ref="S15:T15" si="1">SUM(S2:S14)</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>